<commit_message>
Added disposal excel and receipt excel
</commit_message>
<xml_diff>
--- a/Warehouse/Resources/Disposal.xlsx
+++ b/Warehouse/Resources/Disposal.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Поступление" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,9 +19,84 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>Отчёт о движении продуктов</t>
+  </si>
+  <si>
+    <t>Период: 2023-10-07 - 2023-10-31</t>
+  </si>
+  <si>
+    <t>ОАО Гомельский Мясокомбинат</t>
+  </si>
+  <si>
+    <t>Адрес: Гомель, ул. Ильича, 2</t>
+  </si>
+  <si>
+    <t>Номер заказа</t>
+  </si>
+  <si>
+    <t>Поставщик</t>
+  </si>
+  <si>
+    <t>Сотрудник</t>
+  </si>
+  <si>
+    <t>Сумма</t>
+  </si>
+  <si>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>Тип</t>
+  </si>
+  <si>
+    <t>Товары</t>
+  </si>
+  <si>
+    <t>40002</t>
+  </si>
+  <si>
+    <t>Нетушки</t>
+  </si>
+  <si>
+    <t>лебенков</t>
+  </si>
+  <si>
+    <t>157500</t>
+  </si>
+  <si>
+    <t>27.10.2023 00:00:00</t>
+  </si>
+  <si>
+    <t>Поступление</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>40003</t>
+  </si>
+  <si>
+    <t>18500</t>
+  </si>
+  <si>
+    <t>50002</t>
+  </si>
+  <si>
+    <t>193025</t>
+  </si>
+  <si>
+    <t>28.10.2023 00:00:00</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +121,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +421,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.975940159389" customWidth="1"/>
+    <col min="2" max="2" width="11.4898910522461" customWidth="1"/>
+    <col min="3" max="3" width="11.172741481236" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.4565015520368" customWidth="1"/>
+    <col min="6" max="6" width="13.309924534389" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+  </mergeCells>
+  <pageSetup orientation="landscape"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added last excel output and added date period validation
</commit_message>
<xml_diff>
--- a/Warehouse/Resources/Disposal.xlsx
+++ b/Warehouse/Resources/Disposal.xlsx
@@ -63,7 +63,7 @@
     <t>Продукты</t>
   </si>
   <si>
-    <t>70005</t>
+    <t>80003</t>
   </si>
   <si>
     <t>Сбербанк</t>
@@ -72,7 +72,7 @@
     <t>лебенков</t>
   </si>
   <si>
-    <t>5000</t>
+    <t>819</t>
   </si>
   <si>
     <t>01.11.2023 00:00:00</t>
@@ -81,10 +81,10 @@
     <t>Выбытие</t>
   </si>
   <si>
-    <t>Докторская</t>
-  </si>
-  <si>
-    <t>70006</t>
+    <t>Волковыское</t>
+  </si>
+  <si>
+    <t>Составил: _______________</t>
   </si>
 </sst>
 </file>
@@ -131,10 +131,10 @@
   <cellXfs count="5">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
@@ -418,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,7 +430,7 @@
     <col min="4" max="4" width="9.140625" customWidth="1" style="1"/>
     <col min="5" max="5" width="19.4565015520368" customWidth="1" style="1"/>
     <col min="6" max="6" width="9.68725040980748" customWidth="1" style="1"/>
-    <col min="7" max="7" width="12.0177928379604" customWidth="1" style="1"/>
+    <col min="7" max="7" width="13.5585294451032" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -548,15 +548,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
     <row r="7">
       <c r="A7" s="4" t="s">
         <v>5</v>
@@ -603,27 +594,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
+    <row r="10">
+      <c r="A10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>